<commit_message>
Deploying to main from @ electrified/rcbus-opl3@6dc36e7be147e4cae15e6f13cab98d536f6d43da 🚀
</commit_message>
<xml_diff>
--- a/BoM/Positional/rcbus-opl3-bom.xlsx
+++ b/BoM/Positional/rcbus-opl3-bom.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="247">
   <si>
     <t>Row</t>
   </si>
@@ -182,7 +182,7 @@
     <t>0.9500</t>
   </si>
   <si>
-    <t>Net-(U1-AOUT),GND</t>
+    <t>GND,Net-(U1-AOUT)</t>
   </si>
   <si>
     <t>Default</t>
@@ -242,10 +242,10 @@
     <t>90.0000</t>
   </si>
   <si>
-    <t>+5V,GND</t>
-  </si>
-  <si>
-    <t>Default,vcc</t>
+    <t>GND,+5V</t>
+  </si>
+  <si>
+    <t>vcc,Default</t>
   </si>
   <si>
     <t>4</t>
@@ -392,7 +392,7 @@
     <t>14.4000</t>
   </si>
   <si>
-    <t>+5V,Net-(JP1-Pin_5),Net-(JP1-Pin_11),Net-(JP1-Pin_9),Net-(JP1-Pin_7),Net-(JP1-Pin_1),Net-(JP1-Pin_3)</t>
+    <t>Net-(JP1-Pin_3),Net-(JP1-Pin_1),Net-(JP1-Pin_7),Net-(JP1-Pin_5),Net-(JP1-Pin_11),+5V,Net-(JP1-Pin_9)</t>
   </si>
   <si>
     <t>8</t>
@@ -428,10 +428,10 @@
     <t>98.2200</t>
   </si>
   <si>
-    <t>unconnected-(P1-Pin_35-Pad35),/D0,unconnected-(P1-Pin_21-Pad21),/D6,/D7,/~{IORQ},/A6,/~{RESET},+5V,unconnected-(P1-Pin_1-Pad1),unconnected-(P1-Pin_7-Pad7),/D5,unconnected-(P1-Pin_4-Pad4),/D4,unconnected-(P1-Pin_2-Pad2),/D1,/A0,GND,/~{INT},/A7,unconnected-(P1-Pin_38-Pad38),/D2,unconnected-(P1-Pin_6-Pad6),unconnected-(P1-Pin_37-Pad37),/A4,/A1,/A5,unconnected-(P1-Pin_8-Pad8),unconnected-(P1-Pin_36-Pad36),/A3,unconnected-(P1-Pin_3-Pad3),unconnected-(P1-Pin_23-Pad23),unconnected-(P1-Pin_5-Pad5),unconnected-(P1-Pin_39-Pad39),/~{WR},/A2,unconnected-(P1-Pin_19-Pad19),/D3,/~{RD}</t>
-  </si>
-  <si>
-    <t>~{RD}</t>
+    <t>unconnected-(P1-Pin_36-Pad36),/A6,/A7,/~{WR},/A4,/D4,/D0,/D1,unconnected-(P1-Pin_23-Pad23),GND,/A2,unconnected-(P1-Pin_3-Pad3),/D5,unconnected-(P1-Pin_4-Pad4),unconnected-(P1-Pin_35-Pad35),/D3,unconnected-(P1-Pin_38-Pad38),/D2,unconnected-(P1-Pin_8-Pad8),/~{RD},/D6,unconnected-(P1-Pin_39-Pad39),unconnected-(P1-Pin_1-Pad1),unconnected-(P1-Pin_21-Pad21),unconnected-(P1-Pin_37-Pad37),unconnected-(P1-Pin_2-Pad2),unconnected-(P1-Pin_7-Pad7),unconnected-(P1-Pin_19-Pad19),/D7,/A0,unconnected-(P1-Pin_5-Pad5),/A1,unconnected-(P1-Pin_6-Pad6),/A3,/~{INT},/A5,/~{IORQ},+5V,/~{RESET}</t>
+  </si>
+  <si>
+    <t>~{RESET}</t>
   </si>
   <si>
     <t>9</t>
@@ -500,7 +500,7 @@
     <t>6.7230</t>
   </si>
   <si>
-    <t>Net-(CON1-PadT),GND</t>
+    <t>GND,Net-(CON1-PadT)</t>
   </si>
   <si>
     <t>12</t>
@@ -542,10 +542,10 @@
     <t>12.0300</t>
   </si>
   <si>
-    <t>/~{IORQ},/A3,/A6,GND,/A7,Net-(JP1-Pin_5),+5V,Net-(JP1-Pin_11),/~{CS},/A2,Net-(JP1-Pin_9),/A4,Net-(JP1-Pin_7),Net-(JP1-Pin_1),/A5,Net-(JP1-Pin_3)</t>
-  </si>
-  <si>
-    <t>A5,Net-(JP1-Pin_3)</t>
+    <t>GND,Net-(JP1-Pin_3),/A2,/A3,Net-(JP1-Pin_1),Net-(JP1-Pin_7),/A6,/A7,Net-(JP1-Pin_5),/A5,/A4,Net-(JP1-Pin_11),/~{IORQ},+5V,Net-(JP1-Pin_9),/~{CS}</t>
+  </si>
+  <si>
+    <t>~{CS}</t>
   </si>
   <si>
     <t>13</t>
@@ -584,10 +584,7 @@
     <t>8.2200</t>
   </si>
   <si>
-    <t>/R,Net-(U2B--),GND,/L,+5V,/AUDIO_CH1,/AUDIO_CH2,Net-(U1-MP),Net-(U1-AOUT),Net-(U1-CV)</t>
-  </si>
-  <si>
-    <t>AUDIO_CH2,Net-(U1-MP),Net-(U1-AOUT),Net-(U1-CV)</t>
+    <t>GND,/AUDIO_CH2,/L,Net-(U1-MP),Net-(U2B--),Net-(U1-CV),/AUDIO_CH1,Net-(U1-AOUT),+5V,/R</t>
   </si>
   <si>
     <t>14</t>
@@ -617,10 +614,10 @@
     <t>9.4900</t>
   </si>
   <si>
-    <t>/DOAB,Net-(U1-SWIN),GND,/DAC_CLK,unconnected-(U1-TST2-Pad15),/SMPAC,+5V,/AUDIO_CH1,/AUDIO_CH2,Net-(U1-MP),Net-(U1-AOUT),Net-(U1-CV),/SMPBD</t>
-  </si>
-  <si>
-    <t>SMPBD</t>
+    <t>GND,/AUDIO_CH2,Net-(U1-MP),/AUDIO_CH1,Net-(U1-CV),/SMPAC,/DAC_CLK,Net-(U1-SWIN),Net-(U1-AOUT),/DOAB,+5V,/SMPBD,unconnected-(U1-TST2-Pad15)</t>
+  </si>
+  <si>
+    <t>SMPBD,unconnected-(U1-TST2-Pad15)</t>
   </si>
   <si>
     <t>15</t>
@@ -650,7 +647,7 @@
     <t>14.5200</t>
   </si>
   <si>
-    <t>/DOAB,/D0,/D6,/D7,/~{RESET},+5V,/SMPAC,/D5,unconnected-(U4-TEST-Pad9),/SMPBD,/D4,/D1,/A0,GND,unconnected-(U4-DOCD-Pad22),/CLK,/D2,/~{CS},/A1,/DAC_CLK,unconnected-(U4-~{IRQ}-Pad2),/~{WR},/D3,/~{RD}</t>
+    <t>/~{WR},/D4,/SMPAC,/D0,/D1,/~{CS},GND,/D5,/D3,/DAC_CLK,/DOAB,/D2,/~{RD},/D6,/D7,/A0,unconnected-(U4-TEST-Pad9),/SMPBD,/A1,unconnected-(U4-DOCD-Pad22),+5V,unconnected-(U4-~{IRQ}-Pad2),/CLK,/~{RESET}</t>
   </si>
   <si>
     <t>16</t>
@@ -692,10 +689,10 @@
     <t>6.0000</t>
   </si>
   <si>
-    <t>+5V,GND,/CLK</t>
-  </si>
-  <si>
-    <t>CLK</t>
+    <t>GND,/CLK,+5V</t>
+  </si>
+  <si>
+    <t>CLK,+5V</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -1303,7 +1300,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1337,13 +1334,13 @@
     </row>
     <row r="2" spans="1:32">
       <c r="C2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>228</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F2" s="3">
         <v>16</v>
@@ -1351,41 +1348,41 @@
     </row>
     <row r="3" spans="1:32">
       <c r="C3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>230</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="C4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="C5" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>234</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1393,13 +1390,13 @@
     </row>
     <row r="6" spans="1:32">
       <c r="C6" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="3">
         <v>32</v>
@@ -2189,7 +2186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="165" customHeight="1">
+    <row r="16" spans="1:32" ht="180" customHeight="1">
       <c r="A16" s="9" t="s">
         <v>125</v>
       </c>
@@ -2768,7 +2765,7 @@
         <v>188</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="AE21" s="6" t="s">
         <v>75</v>
@@ -2779,25 +2776,25 @@
     </row>
     <row r="22" spans="1:32" ht="45" customHeight="1">
       <c r="A22" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>167</v>
@@ -2830,13 +2827,13 @@
         <v>44</v>
       </c>
       <c r="R22" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="S22" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="S22" s="11" t="s">
+      <c r="T22" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="T22" s="11" t="s">
-        <v>196</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>73</v>
@@ -2854,19 +2851,19 @@
         <v>51</v>
       </c>
       <c r="Z22" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA22" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="AA22" s="11" t="s">
+      <c r="AB22" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC22" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="AB22" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="AC22" s="10" t="s">
+      <c r="AD22" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="AD22" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="AE22" s="10" t="s">
         <v>75</v>
@@ -2877,25 +2874,25 @@
     </row>
     <row r="23" spans="1:32" ht="60" customHeight="1">
       <c r="A23" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>202</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>103</v>
       </c>
       <c r="E23" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>167</v>
@@ -2928,13 +2925,13 @@
         <v>44</v>
       </c>
       <c r="R23" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="S23" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="S23" s="7" t="s">
+      <c r="T23" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="U23" s="7" t="s">
         <v>63</v>
@@ -2952,16 +2949,16 @@
         <v>51</v>
       </c>
       <c r="Z23" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA23" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="AA23" s="7" t="s">
+      <c r="AB23" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC23" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="AB23" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="AC23" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="AD23" s="6" t="s">
         <v>137</v>
@@ -2975,28 +2972,28 @@
     </row>
     <row r="24" spans="1:32">
       <c r="A24" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>217</v>
-      </c>
       <c r="H24" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>32</v>
@@ -3008,7 +3005,7 @@
         <v>40</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M24" s="11" t="s">
         <v>42</v>
@@ -3026,13 +3023,13 @@
         <v>44</v>
       </c>
       <c r="R24" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="S24" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="S24" s="11" t="s">
+      <c r="T24" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="T24" s="11" t="s">
-        <v>221</v>
       </c>
       <c r="U24" s="11" t="s">
         <v>73</v>
@@ -3050,19 +3047,19 @@
         <v>51</v>
       </c>
       <c r="Z24" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA24" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="AA24" s="11" t="s">
+      <c r="AB24" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="AC24" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="AB24" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="AC24" s="10" t="s">
+      <c r="AD24" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="AD24" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="AE24" s="10" t="s">
         <v>75</v>
@@ -3094,27 +3091,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>